<commit_message>
SSDM-8226 Added first version of number field search criteria test.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210C2F31-02BD-6F4A-A754-3A042CFDC2A1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0489C15-EDA3-DE4C-9C61-E7C064D1D088}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="840" windowWidth="31100" windowHeight="22120" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="1280" yWindow="460" windowWidth="27520" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="160">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -503,6 +503,9 @@
   </si>
   <si>
     <t>clazz.getName()</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -1752,10 +1755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD85"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3670,7 +3673,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="b">
         <v>0</v>
       </c>
@@ -3687,7 +3690,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="b">
         <v>0</v>
       </c>
@@ -3704,7 +3707,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="b">
         <v>0</v>
       </c>
@@ -3721,7 +3724,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="b">
         <v>0</v>
       </c>
@@ -3738,7 +3741,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="b">
         <v>0</v>
       </c>
@@ -3755,7 +3758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="b">
         <v>1</v>
       </c>
@@ -3772,7 +3775,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="b">
         <v>1</v>
       </c>
@@ -3789,7 +3792,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="b">
         <v>1</v>
       </c>
@@ -3806,7 +3809,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="b">
         <v>1</v>
       </c>
@@ -3823,7 +3826,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="b">
         <v>1</v>
       </c>
@@ -3840,7 +3843,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="b">
         <v>1</v>
       </c>
@@ -3856,8 +3859,11 @@
       <c r="E123" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F123" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="b">
         <v>0</v>
       </c>
@@ -3874,7 +3880,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="9" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
SSDM-8226 Completed the number field verification test.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0489C15-EDA3-DE4C-9C61-E7C064D1D088}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0DCB80-3241-814B-8C82-8E26ADF6B91F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="460" windowWidth="27520" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="160">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1758,7 +1758,7 @@
   <dimension ref="A1:F125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="F124" sqref="F124"/>
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3842,6 +3842,9 @@
       <c r="E122" t="s">
         <v>56</v>
       </c>
+      <c r="F122" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="b">

</xml_diff>

<commit_message>
SSDM-8226 Added collection and date field search criteria tests.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0DCB80-3241-814B-8C82-8E26ADF6B91F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF7186A-4C68-374C-B764-55697C3C76C0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="460" windowWidth="27520" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="160">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1757,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="F123" sqref="F123"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3791,6 +3791,9 @@
       <c r="E119" t="s">
         <v>54</v>
       </c>
+      <c r="F119" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="b">
@@ -3807,6 +3810,9 @@
       </c>
       <c r="E120" t="s">
         <v>73</v>
+      </c>
+      <c r="F120" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SSDM-8226 Updates covered criteria document.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF7186A-4C68-374C-B764-55697C3C76C0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F706245-3E9A-CA43-824B-D937202A4639}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="160">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -585,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -600,6 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1757,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F120" sqref="F120"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2585,58 +2586,67 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="b">
-        <v>0</v>
-      </c>
-      <c r="B49" t="s">
-        <v>137</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D49" t="s">
+    <row r="49" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="b">
-        <v>0</v>
-      </c>
-      <c r="B50" t="s">
-        <v>137</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="F49" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="b">
-        <v>0</v>
-      </c>
-      <c r="B51" t="s">
-        <v>137</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="F50" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="b">
         <v>0</v>
       </c>
@@ -2653,41 +2663,47 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="b">
-        <v>0</v>
-      </c>
-      <c r="B53" t="s">
-        <v>137</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D53" t="s">
+    <row r="53" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="b">
-        <v>0</v>
-      </c>
-      <c r="B54" t="s">
-        <v>137</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="F53" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="b">
         <v>0</v>
       </c>
@@ -2704,7 +2720,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="b">
         <v>0</v>
       </c>
@@ -2721,7 +2737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="b">
         <v>0</v>
       </c>
@@ -2738,7 +2754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="b">
         <v>0</v>
       </c>
@@ -2755,7 +2771,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="b">
         <v>0</v>
       </c>
@@ -2772,7 +2788,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="b">
         <v>0</v>
       </c>
@@ -2789,7 +2805,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="b">
         <v>0</v>
       </c>
@@ -2806,7 +2822,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="b">
         <v>0</v>
       </c>
@@ -2823,58 +2839,67 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="b">
-        <v>0</v>
-      </c>
-      <c r="B63" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D63" t="s">
+    <row r="63" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="b">
-        <v>0</v>
-      </c>
-      <c r="B64" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="F63" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="b">
-        <v>0</v>
-      </c>
-      <c r="B65" t="s">
-        <v>137</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="F64" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="b">
         <v>0</v>
       </c>
@@ -2891,7 +2916,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="b">
         <v>0</v>
       </c>
@@ -2908,449 +2933,527 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" t="b">
-        <v>0</v>
-      </c>
-      <c r="B68" t="s">
-        <v>137</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D68" t="s">
+    <row r="68" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" t="b">
-        <v>0</v>
-      </c>
-      <c r="B69" t="s">
-        <v>137</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="F68" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" t="b">
-        <v>0</v>
-      </c>
-      <c r="B70" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="F69" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" t="b">
-        <v>0</v>
-      </c>
-      <c r="B71" t="s">
-        <v>137</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="F70" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" t="b">
-        <v>0</v>
-      </c>
-      <c r="B72" t="s">
-        <v>137</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="F71" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" t="b">
-        <v>0</v>
-      </c>
-      <c r="B73" t="s">
-        <v>137</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="F72" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" t="b">
-        <v>0</v>
-      </c>
-      <c r="B74" t="s">
-        <v>137</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="F73" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" t="b">
-        <v>0</v>
-      </c>
-      <c r="B75" t="s">
-        <v>137</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="F74" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" t="b">
-        <v>0</v>
-      </c>
-      <c r="B76" t="s">
-        <v>137</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="F75" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" t="b">
-        <v>0</v>
-      </c>
-      <c r="B77" t="s">
-        <v>137</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="F76" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" t="b">
-        <v>0</v>
-      </c>
-      <c r="B78" t="s">
-        <v>137</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="F77" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" t="b">
-        <v>0</v>
-      </c>
-      <c r="B79" t="s">
-        <v>137</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="F78" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" t="b">
-        <v>0</v>
-      </c>
-      <c r="B80" t="s">
-        <v>137</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="F79" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" t="b">
-        <v>0</v>
-      </c>
-      <c r="B81" t="s">
-        <v>137</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="F80" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" t="b">
-        <v>0</v>
-      </c>
-      <c r="B82" t="s">
-        <v>137</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="F81" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" t="b">
-        <v>0</v>
-      </c>
-      <c r="B83" t="s">
-        <v>137</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="F82" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" t="b">
-        <v>0</v>
-      </c>
-      <c r="B84" t="s">
-        <v>137</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="F83" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" t="b">
-        <v>0</v>
-      </c>
-      <c r="B85" t="s">
-        <v>137</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="F84" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" t="b">
-        <v>0</v>
-      </c>
-      <c r="B86" t="s">
-        <v>137</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="F85" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" t="b">
-        <v>0</v>
-      </c>
-      <c r="B87" t="s">
-        <v>137</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="F86" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" t="b">
-        <v>0</v>
-      </c>
-      <c r="B88" t="s">
-        <v>137</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="F87" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" t="b">
-        <v>0</v>
-      </c>
-      <c r="B89" t="s">
-        <v>137</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="F88" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" t="b">
-        <v>0</v>
-      </c>
-      <c r="B90" t="s">
-        <v>137</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="F89" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" t="b">
-        <v>0</v>
-      </c>
-      <c r="B91" t="s">
-        <v>137</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="F90" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" t="b">
-        <v>0</v>
-      </c>
-      <c r="B92" t="s">
-        <v>137</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="F91" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" t="b">
-        <v>0</v>
-      </c>
-      <c r="B93" t="s">
-        <v>137</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="F92" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="b">
         <v>1</v>
       </c>
@@ -3367,7 +3470,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="b">
         <v>1</v>
       </c>
@@ -3384,7 +3487,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="b">
         <v>0</v>
       </c>
@@ -3775,43 +3878,43 @@
         <v>52</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" t="b">
+    <row r="119" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C119" t="s">
-        <v>137</v>
-      </c>
-      <c r="D119" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E119" t="s">
+      <c r="C119" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D119" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E119" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F119" t="s">
+      <c r="F119" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A120" t="b">
+    <row r="120" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C120" t="s">
-        <v>137</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E120" t="s">
+      <c r="C120" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D120" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E120" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F120" t="s">
+      <c r="F120" s="1" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3832,43 +3935,43 @@
         <v>71</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122" t="b">
+    <row r="122" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C122" t="s">
-        <v>137</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E122" t="s">
+      <c r="C122" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D122" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E122" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F122" t="s">
+      <c r="F122" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123" t="b">
+    <row r="123" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C123" t="s">
-        <v>137</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E123" t="s">
+      <c r="C123" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D123" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E123" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F123" t="s">
+      <c r="F123" s="1" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SSDM-8226 Added own space, project, experiment type and experiment instead of presuming that there is one.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F706245-3E9A-CA43-824B-D937202A4639}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87BF818-E74E-7B44-9435-4EB76F5EA9C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -506,6 +506,12 @@
   </si>
   <si>
     <t>+</t>
+  </si>
+  <si>
+    <t>Tested</t>
+  </si>
+  <si>
+    <t>Untested</t>
   </si>
 </sst>
 </file>
@@ -1756,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1768,9 +1774,10 @@
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="92.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>154</v>
       </c>
@@ -1786,8 +1793,14 @@
       <c r="E1" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="b">
         <v>0</v>
       </c>
@@ -1804,7 +1817,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -1821,7 +1834,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -1838,7 +1851,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -1855,7 +1868,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="b">
         <v>0</v>
       </c>
@@ -1872,7 +1885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -1889,7 +1902,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -1906,7 +1919,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -1923,7 +1936,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -1940,7 +1953,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -1957,7 +1970,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -1974,7 +1987,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="b">
         <v>0</v>
       </c>
@@ -1991,7 +2004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="b">
         <v>0</v>
       </c>
@@ -2008,7 +2021,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="b">
         <v>0</v>
       </c>
@@ -2025,7 +2038,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
SSDM-8226 Separated DB connections, so that DB initialisation, DB cleanup and each test are using their own DB connection.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87BF818-E74E-7B44-9435-4EB76F5EA9C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA4B405-35F6-764B-B45F-3494E9F947ED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1764,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2599,7 +2599,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="b">
         <v>0</v>
       </c>
@@ -2618,8 +2618,11 @@
       <c r="F49" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G49" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="b">
         <v>0</v>
       </c>
@@ -2639,7 +2642,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="b">
         <v>0</v>
       </c>
@@ -2659,7 +2662,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="b">
         <v>0</v>
       </c>
@@ -2676,7 +2679,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="b">
         <v>0</v>
       </c>
@@ -2696,7 +2699,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="b">
         <v>0</v>
       </c>
@@ -2716,7 +2719,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="b">
         <v>0</v>
       </c>
@@ -2733,7 +2736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="b">
         <v>0</v>
       </c>
@@ -2750,7 +2753,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="b">
         <v>0</v>
       </c>
@@ -2767,7 +2770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="b">
         <v>0</v>
       </c>
@@ -2784,7 +2787,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="b">
         <v>0</v>
       </c>
@@ -2801,7 +2804,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="b">
         <v>0</v>
       </c>
@@ -2818,7 +2821,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="b">
         <v>0</v>
       </c>
@@ -2835,7 +2838,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="b">
         <v>0</v>
       </c>
@@ -2852,7 +2855,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="b">
         <v>0</v>
       </c>
@@ -2872,7 +2875,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="b">
         <v>0</v>
       </c>
@@ -3206,7 +3209,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="b">
         <v>0</v>
       </c>
@@ -3226,7 +3229,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="b">
         <v>0</v>
       </c>
@@ -3246,7 +3249,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="b">
         <v>0</v>
       </c>
@@ -3266,7 +3269,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="b">
         <v>0</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="b">
         <v>0</v>
       </c>
@@ -3306,7 +3309,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="86" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="b">
         <v>0</v>
       </c>
@@ -3326,7 +3329,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="b">
         <v>0</v>
       </c>
@@ -3346,7 +3349,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="88" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="b">
         <v>0</v>
       </c>
@@ -3366,7 +3369,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="89" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="b">
         <v>0</v>
       </c>
@@ -3386,7 +3389,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="90" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="b">
         <v>0</v>
       </c>
@@ -3406,7 +3409,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="b">
         <v>0</v>
       </c>
@@ -3426,7 +3429,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="92" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="b">
         <v>0</v>
       </c>
@@ -3446,7 +3449,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="b">
         <v>0</v>
       </c>
@@ -3466,7 +3469,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="b">
         <v>1</v>
       </c>
@@ -3483,7 +3486,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="b">
         <v>1</v>
       </c>
@@ -3500,7 +3503,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="b">
         <v>0</v>
       </c>
@@ -3516,8 +3519,14 @@
       <c r="E96" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G96" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="b">
         <v>0</v>
       </c>
@@ -3533,8 +3542,14 @@
       <c r="E97" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G97" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="b">
         <v>0</v>
       </c>
@@ -3550,8 +3565,14 @@
       <c r="E98" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G98" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="b">
         <v>0</v>
       </c>
@@ -3567,8 +3588,14 @@
       <c r="E99" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G99" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="9" t="b">
         <v>1</v>
       </c>
@@ -3585,7 +3612,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="9" t="b">
         <v>1</v>
       </c>
@@ -3602,7 +3629,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="b">
         <v>0</v>
       </c>
@@ -3619,7 +3646,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="b">
         <v>0</v>
       </c>
@@ -3636,7 +3663,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="b">
         <v>0</v>
       </c>
@@ -3653,7 +3680,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="b">
         <v>0</v>
       </c>
@@ -3670,7 +3697,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="9" t="b">
         <v>0</v>
       </c>
@@ -3687,7 +3714,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="b">
         <v>0</v>
       </c>
@@ -3704,7 +3731,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="9" t="b">
         <v>0</v>
       </c>
@@ -3721,7 +3748,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="b">
         <v>0</v>
       </c>
@@ -3738,7 +3765,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="b">
         <v>0</v>
       </c>
@@ -3755,7 +3782,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="b">
         <v>0</v>
       </c>
@@ -3772,7 +3799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
SSDM-8226 Added test for modification date.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA4B405-35F6-764B-B45F-3494E9F947ED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F597C9-9DA2-9649-9D17-E0164B2C61BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1764,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2698,6 +2698,9 @@
       <c r="F53" s="1" t="s">
         <v>159</v>
       </c>
+      <c r="G53" s="1" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="54" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="b">
@@ -2718,6 +2721,9 @@
       <c r="F54" s="1" t="s">
         <v>159</v>
       </c>
+      <c r="G54" s="1" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="b">
@@ -2895,7 +2901,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="b">
         <v>0</v>
       </c>
@@ -2915,7 +2921,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="b">
         <v>0</v>
       </c>
@@ -2932,7 +2938,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="b">
         <v>0</v>
       </c>
@@ -2949,7 +2955,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="b">
         <v>0</v>
       </c>
@@ -2968,8 +2974,11 @@
       <c r="F68" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G68" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="b">
         <v>0</v>
       </c>
@@ -2989,7 +2998,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="b">
         <v>0</v>
       </c>
@@ -3009,7 +3018,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="b">
         <v>0</v>
       </c>
@@ -3029,7 +3038,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="b">
         <v>0</v>
       </c>
@@ -3048,8 +3057,11 @@
       <c r="F72" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G72" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="b">
         <v>0</v>
       </c>
@@ -3069,7 +3081,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="b">
         <v>0</v>
       </c>
@@ -3089,7 +3101,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="b">
         <v>0</v>
       </c>
@@ -3109,7 +3121,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="b">
         <v>0</v>
       </c>
@@ -3129,7 +3141,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="b">
         <v>0</v>
       </c>
@@ -3149,7 +3161,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="b">
         <v>0</v>
       </c>
@@ -3169,7 +3181,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="b">
         <v>0</v>
       </c>
@@ -3189,7 +3201,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
SSDM-8226 In progress of adding test for all fields.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F597C9-9DA2-9649-9D17-E0164B2C61BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB72D2D-8F76-8942-894B-54D21634B6FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1764,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3828,7 +3828,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="b">
         <v>0</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="b">
         <v>0</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="b">
         <v>0</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="b">
         <v>0</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="b">
         <v>0</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="b">
         <v>1</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="119" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="b">
         <v>1</v>
       </c>
@@ -3949,8 +3949,11 @@
       <c r="F119" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G119" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="b">
         <v>1</v>
       </c>
@@ -3969,8 +3972,11 @@
       <c r="F120" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G120" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="b">
         <v>1</v>
       </c>
@@ -3987,7 +3993,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="122" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="b">
         <v>1</v>
       </c>
@@ -4007,7 +4013,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="123" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="b">
         <v>1</v>
       </c>
@@ -4026,8 +4032,11 @@
       <c r="F123" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G123" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="b">
         <v>0</v>
       </c>
@@ -4044,7 +4053,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="9" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
SSDM-8226 Implemented translation of a query by ID field.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB72D2D-8F76-8942-894B-54D21634B6FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AE7365-EEF7-0B46-B133-7EC06199F4DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -591,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -607,6 +607,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1764,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2861,81 +2864,87 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D63" s="1" t="s">
+    <row r="63" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D64" s="1" t="s">
+      <c r="F63" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D64" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C65" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D65" s="1" t="s">
+      <c r="F64" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D65" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" t="b">
-        <v>0</v>
-      </c>
-      <c r="B66" t="s">
-        <v>137</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="F65" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="1" t="s">
         <v>76</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -2978,63 +2987,63 @@
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D69" s="1" t="s">
+    <row r="69" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D70" s="1" t="s">
+      <c r="F69" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D70" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F70" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D71" s="1" t="s">
+      <c r="F70" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D71" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F71" s="12" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3061,423 +3070,423 @@
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D73" s="1" t="s">
+    <row r="73" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D73" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D74" s="1" t="s">
+      <c r="F73" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D74" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F74" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C75" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D75" s="1" t="s">
+      <c r="F74" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D75" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C76" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D76" s="1" t="s">
+      <c r="F75" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D76" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D77" s="1" t="s">
+      <c r="F76" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D77" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F77" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D78" s="1" t="s">
+      <c r="F77" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D78" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D79" s="1" t="s">
+      <c r="F78" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C79" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D79" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E79" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C80" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D80" s="1" t="s">
+      <c r="F79" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E80" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C81" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D81" s="1" t="s">
+      <c r="F80" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D81" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E81" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C82" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D82" s="1" t="s">
+      <c r="F81" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D82" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E82" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C83" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D83" s="1" t="s">
+      <c r="F82" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D83" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E83" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C84" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D84" s="1" t="s">
+      <c r="F83" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D84" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E84" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D85" s="1" t="s">
+      <c r="F84" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D85" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E85" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F85" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D86" s="1" t="s">
+      <c r="F85" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D86" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="E86" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D87" s="1" t="s">
+      <c r="F86" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D87" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="E87" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D88" s="1" t="s">
+      <c r="F87" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D88" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E88" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C89" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D89" s="1" t="s">
+      <c r="F88" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D89" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E89" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D90" s="1" t="s">
+      <c r="F89" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D90" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="E90" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C91" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D91" s="1" t="s">
+      <c r="F90" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D91" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E91" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D92" s="1" t="s">
+      <c r="F91" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D92" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="E92" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D93" s="1" t="s">
+      <c r="F92" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D93" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E93" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="F93" s="1" t="s">
+      <c r="F93" s="12" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3515,95 +3524,95 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" t="b">
-        <v>0</v>
-      </c>
-      <c r="B96" t="s">
+    <row r="96" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D96" s="6" t="s">
+      <c r="D96" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G96" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" t="b">
-        <v>0</v>
-      </c>
-      <c r="B97" t="s">
+      <c r="G96" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D97" s="6" t="s">
+      <c r="D97" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G97" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" t="b">
-        <v>0</v>
-      </c>
-      <c r="B98" t="s">
+      <c r="G97" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D98" s="6" t="s">
+      <c r="D98" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="1" t="s">
         <v>83</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G98" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" t="b">
-        <v>0</v>
-      </c>
-      <c r="B99" t="s">
+      <c r="G98" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D99" s="6" t="s">
+      <c r="D99" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G99" s="1" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SSDM-8226 Removed not tested translators from the criteria to condition translator map.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478D701D-7032-2243-A878-D54C4D7A689D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C026BF-A384-3547-B8E8-54B3FF1343A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -591,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -610,6 +610,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1767,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G119" sqref="G119"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3650,21 +3651,27 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B102" s="9" t="s">
+    <row r="102" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B102" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="C102" s="9" t="s">
+      <c r="C102" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D102" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E102" s="9" t="s">
+      <c r="D102" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E102" s="14" t="s">
         <v>72</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SSDM-8583 Implemented the first version of a query by a property.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C026BF-A384-3547-B8E8-54B3FF1343A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60B3712-3CE4-4540-9471-9DA100033F87}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -1768,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
SSDM-8583 Expanded string property test.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60B3712-3CE4-4540-9471-9DA100033F87}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18998A61-F8E5-AB4E-BAEA-1C89011C1815}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1768,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2666,21 +2666,27 @@
         <v>159</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" t="b">
-        <v>0</v>
-      </c>
-      <c r="B52" t="s">
-        <v>137</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D52" t="s">
+    <row r="52" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="1" t="s">
         <v>57</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2848,21 +2854,27 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" t="b">
-        <v>0</v>
-      </c>
-      <c r="B62" t="s">
-        <v>137</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D62" t="s">
+    <row r="62" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="1" t="s">
         <v>58</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -3071,23 +3083,26 @@
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D73" s="12" t="s">
+    <row r="73" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F73" s="12" t="s">
+      <c r="F73" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G73" s="1" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SSDM-8583 Added a test for combinations (with logical AND and OR) of search criteria.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18998A61-F8E5-AB4E-BAEA-1C89011C1815}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F17A658-E694-DE40-A323-3D1D81D3D940}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -1768,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:XFD67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2960,21 +2960,27 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" t="b">
-        <v>0</v>
-      </c>
-      <c r="B67" t="s">
-        <v>137</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D67" t="s">
+    <row r="67" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="1" t="s">
         <v>67</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SSDM-8226 Implemented another succeeding test in SampleTypeSearchManagerDBTest.java: search by listable value.
</commit_message>
<xml_diff>
--- a/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
+++ b/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/criterias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/source/java/ch/ethz/sis/openbis/generic/server/asapi/v3/search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F17A658-E694-DE40-A323-3D1D81D3D940}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22699C39-38FA-BD4A-88A4-7D29F213E976}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="36800" windowHeight="23540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="27460" windowHeight="17540" activeTab="1" xr2:uid="{39EE687D-4414-3747-AFBA-7E58B6CC49A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="162">
   <si>
     <t>ch.ethz.sis.openbis.generic.asapi.v3.dto.operation.search.OperationExecutionSearchCriteria</t>
   </si>
@@ -591,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -611,6 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1768,8 +1769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659BE2D9-7405-F646-AD2E-50E30EAAC445}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:XFD67"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2059,7 +2060,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="b">
         <v>0</v>
       </c>
@@ -2076,7 +2077,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="b">
         <v>0</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="b">
         <v>0</v>
       </c>
@@ -2110,24 +2111,30 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="8" t="s">
+    <row r="20" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="15" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -2144,7 +2151,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -2161,7 +2168,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -2178,7 +2185,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -2195,7 +2202,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -2212,7 +2219,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -2229,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="b">
         <v>1</v>
       </c>
@@ -2246,7 +2253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -2263,7 +2270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="b">
         <v>0</v>
       </c>
@@ -2280,7 +2287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="b">
         <v>0</v>
       </c>
@@ -2297,7 +2304,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="b">
         <v>0</v>
       </c>
@@ -2314,7 +2321,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="b">
         <v>0</v>
       </c>

</xml_diff>